<commit_message>
oka-shujin product_types and codes
</commit_message>
<xml_diff>
--- a/crystania/checklist.xlsx
+++ b/crystania/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/crystania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{229FB34E-3C96-3147-A256-D6F3363CAAAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DFA5DF1-6DF3-A040-96A4-C0A29822DEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{0061518C-7686-BF4D-A945-D57300B57FED}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>product_code</t>
   </si>
   <si>
-    <t>rulebook</t>
-  </si>
-  <si>
     <t>replay</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>Crystania Complete Guidebook</t>
+  </si>
+  <si>
+    <t>box set</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,7 +616,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -637,7 +637,7 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -658,10 +658,10 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -672,19 +672,19 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -704,10 +704,10 @@
         <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -718,19 +718,19 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -750,10 +750,10 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -770,13 +770,13 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -793,13 +793,13 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -816,13 +816,13 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -830,22 +830,22 @@
         <v>1999</v>
       </c>
       <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>